<commit_message>
Generate final market share analysis report with corrected column access
</commit_message>
<xml_diff>
--- a/market_research/data/market_share_analysis_20260214.xlsx
+++ b/market_research/data/market_share_analysis_20260214.xlsx
@@ -528,133 +528,133 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Gingersoft</t>
+          <t>Eats365</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>薑軟件</t>
+          <t>Eats365</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>飯糰</t>
+          <t>Eats365 POS</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="E2" t="n">
-        <v>46</v>
+        <v>4138</v>
       </c>
       <c r="F2" t="n">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="G2" t="n">
-        <v>3.51295</v>
+        <v>2.88889</v>
       </c>
       <c r="H2" t="n">
-        <v>193</v>
+        <v>27</v>
       </c>
       <c r="I2" t="n">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025-09-10T01:27:50Z</t>
+          <t>2026-02-05T16:04:29Z</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>34.76</v>
+        <v>48.21</v>
       </c>
       <c r="L2" t="n">
-        <v>13.59</v>
+        <v>14.86</v>
       </c>
       <c r="M2" t="n">
-        <v>8.31</v>
+        <v>18.08</v>
       </c>
       <c r="N2" t="n">
-        <v>3.75</v>
+        <v>9.75</v>
       </c>
       <c r="O2" t="n">
-        <v>9.109999999999999</v>
+        <v>5.51</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0.3476</v>
+        <v>0.4821</v>
       </c>
       <c r="R2" t="n">
-        <v>196</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DimPOS</t>
+          <t>Gingersoft</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DimPOS</t>
+          <t>薑軟件</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DimOrder</t>
+          <t>飯糰</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F3" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G3" t="n">
-        <v>3.11696</v>
+        <v>3.51295</v>
       </c>
       <c r="H3" t="n">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="I3" t="n">
         <v>100</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2022-06-02T15:27:49Z</t>
+          <t>2025-09-10T01:27:50Z</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>10.87</v>
+        <v>34.76</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>13.59</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>8.31</v>
       </c>
       <c r="N3" t="n">
-        <v>2</v>
+        <v>3.75</v>
       </c>
       <c r="O3" t="n">
-        <v>8.869999999999999</v>
+        <v>9.109999999999999</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>0.1087</v>
+        <v>0.3476</v>
       </c>
       <c r="R3" t="n">
-        <v>61</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4">
@@ -713,7 +713,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q4" t="n">
@@ -726,67 +726,67 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Eats365</t>
+          <t>DoLA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Eats365</t>
+          <t>DoLA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Eats365 POS</t>
+          <t>DoLA Connect</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>4138</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="G5" t="n">
-        <v>2.88889</v>
+        <v>4.7</v>
       </c>
       <c r="H5" t="n">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="I5" t="n">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2026-02-05T16:04:29Z</t>
+          <t>2025-12-12T10:01:25Z</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>48.21</v>
+        <v>15.29</v>
       </c>
       <c r="L5" t="n">
-        <v>14.86</v>
+        <v>4.82</v>
       </c>
       <c r="M5" t="n">
-        <v>18.08</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>9.75</v>
+        <v>6.25</v>
       </c>
       <c r="O5" t="n">
-        <v>5.51</v>
+        <v>4.22</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q5" t="n">
-        <v>0.4821</v>
+        <v>0.1529</v>
       </c>
       <c r="R5" t="n">
-        <v>273</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6">
@@ -845,7 +845,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q6" t="n">
@@ -858,83 +858,83 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DoLA</t>
+          <t>Caterlord</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DoLA</t>
+          <t>Caterlord</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>DoLA Connect</t>
+          <t>餐飲王 HQ</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G7" t="n">
-        <v>4.7</v>
+        <v>5</v>
       </c>
       <c r="H7" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2025-12-12T10:01:25Z</t>
+          <t>2015-11-10T23:48:38Z</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>15.29</v>
+        <v>11.14</v>
       </c>
       <c r="L7" t="n">
-        <v>4.82</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>6.25</v>
+        <v>8</v>
       </c>
       <c r="O7" t="n">
-        <v>4.22</v>
+        <v>3.14</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q7" t="n">
-        <v>0.1529</v>
+        <v>0.1114</v>
       </c>
       <c r="R7" t="n">
-        <v>86</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>OmniWe</t>
+          <t>DimPOS</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OmniWe</t>
+          <t>DimPOS</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Chicks</t>
+          <t>DimOrder</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -944,24 +944,24 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" t="n">
-        <v>4</v>
+        <v>3.11696</v>
       </c>
       <c r="H8" t="n">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="I8" t="n">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2025-08-29T04:04:19Z</t>
+          <t>2022-06-02T15:27:49Z</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>5.74</v>
+        <v>10.87</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -970,37 +970,37 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="O8" t="n">
-        <v>3.24</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>0.0574</v>
+        <v>0.1087</v>
       </c>
       <c r="R8" t="n">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Caterlord</t>
+          <t>OmniWe</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Caterlord</t>
+          <t>OmniWe</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>餐飲王 HQ</t>
+          <t>Chicks</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -1010,47 +1010,47 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I9" t="n">
+        <v>12</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2025-08-29T04:04:19Z</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>5.74</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O9" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>2026-02-14 10:23:49</t>
+        </is>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.0574</v>
+      </c>
+      <c r="R9" t="n">
         <v>32</v>
-      </c>
-      <c r="G9" t="n">
-        <v>5</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>2015-11-10T23:48:38Z</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>11.14</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>8</v>
-      </c>
-      <c r="O9" t="n">
-        <v>3.14</v>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>2026-02-14 10:21:37</t>
-        </is>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.1114</v>
-      </c>
-      <c r="R9" t="n">
-        <v>63</v>
       </c>
     </row>
     <row r="10">
@@ -1105,7 +1105,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q10" t="n">
@@ -1118,17 +1118,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tappo</t>
+          <t>HCTC</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Tappo</t>
+          <t>HCTC</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Gotappo, Tappo</t>
+          <t>HCTC 餐飲</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -1138,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1160,37 +1160,37 @@
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="R11" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>HCTC</t>
+          <t>ezPOS</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>HCTC</t>
+          <t>ezPOS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>HCTC 餐飲</t>
+          <t>ezPOS Biz</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1200,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -1211,9 +1211,13 @@
       <c r="I12" t="n">
         <v>0</v>
       </c>
-      <c r="J12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>2026-02-05T08:34:28Z</t>
+        </is>
+      </c>
       <c r="K12" t="n">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
@@ -1222,37 +1226,37 @@
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="O12" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q12" t="n">
-        <v>0.025</v>
+        <v>0.005</v>
       </c>
       <c r="R12" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ezPOS</t>
+          <t>Tappo</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ezPOS</t>
+          <t>Tappo</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ezPOS Biz</t>
+          <t>Gotappo, Tappo</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1262,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -1273,13 +1277,9 @@
       <c r="I13" t="n">
         <v>0</v>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>2026-02-05T08:34:28Z</t>
-        </is>
-      </c>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
@@ -1288,21 +1288,21 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
         <v>0</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>2026-02-14 10:21:37</t>
+          <t>2026-02-14 10:23:49</t>
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>